<commit_message>
Fixes X minutiae value
Fixes X min value for numbers 7,13 and 14 with approximate guess using
the provided min image.
</commit_message>
<xml_diff>
--- a/TestData/Perfect minutiae/Man Inspection Prints/Worn- done/T_Ale1439795470-Hamster-1-3.xlsx
+++ b/TestData/Perfect minutiae/Man Inspection Prints/Worn- done/T_Ale1439795470-Hamster-1-3.xlsx
@@ -490,7 +490,7 @@
   <dimension ref="A1:V19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -597,9 +597,9 @@
         <f>CONCATENATE('Support Data'!D11,'Support Data'!D12,'Support Data'!D13,'Support Data'!D14)</f>
         <v>464D5200203230000000008A0000012C019000C500C5010000105B12</v>
       </c>
-      <c r="Q2" s="14" t="e">
+      <c r="Q2" s="14" t="str">
         <f>CONCATENATE(P2,P10,'Support Data'!C17)</f>
-        <v>#NUM!</v>
+        <v>464D5200203230000000008A0000012C019000C500C5010000105B12803C00428000806E003B870080AF003D010080CF005080008036008B8C0080B400BD080080FB00D3E90040A500DF9100804D011B9A0080B700E90500806F0145A80080F401106B0080FD0155B80080FA01811D0040D90144850040EE01426F00801700AD91008078008C90000000</v>
       </c>
       <c r="R2" s="14"/>
       <c r="S2" s="14"/>
@@ -839,7 +839,7 @@
         <v>15</v>
       </c>
       <c r="C8" s="12">
-        <v>266.5</v>
+        <v>251.5</v>
       </c>
       <c r="D8">
         <v>211</v>
@@ -855,9 +855,9 @@
         <f>IF(B8='Support Data'!$B$4, 'Support Data'!$C$4, 'Support Data'!$C$3)</f>
         <v>80</v>
       </c>
-      <c r="J8" t="e">
+      <c r="J8" t="str">
         <f t="shared" si="1"/>
-        <v>#NUM!</v>
+        <v>FB</v>
       </c>
       <c r="K8" t="str">
         <f t="shared" si="2"/>
@@ -867,9 +867,9 @@
         <f t="shared" si="3"/>
         <v>E9</v>
       </c>
-      <c r="M8" t="e">
+      <c r="M8" t="str">
         <f>CONCATENATE(I8,J8,'Support Data'!$C$7,K8,L8,'Support Data'!$C$8)</f>
-        <v>#NUM!</v>
+        <v>80FB00D3E900</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
@@ -956,9 +956,9 @@
         <f>CONCATENATE(I10,J10,'Support Data'!$C$7,K10,L10,'Support Data'!$C$8)</f>
         <v>804D011B9A00</v>
       </c>
-      <c r="P10" s="1" t="e">
+      <c r="P10" s="1" t="str">
         <f>CONCATENATE(M2,M3,M4,M5,M6,M7,M8,M9,M10,M11,M12,M13,M14,M15,M16,M17,M18,M19,M20,M21,M22,M23,M24,M25,M26,M27,M28,M29,M30,M31,M32,M33,M34,M35,M36,M37,M38,M39,M40,M41,M42,M43,M44,M45,M46,M47,M48,M49,M50,M51,M52,M53,M54,M55,M56,M57,M58,M59,M60,M61,M62,M63,M64,M65,M66,M67,M68,M69,M70,M71,M72,M73,M74,M75,M76,M77,M78,M79,M80,M81,M82,M83,M84,M85,M86,M87,M88,M89,M90,M91,M92,M93,M94,M95,M96,M97,M98,M99,M100,M101,M102,M103,M104,M105,M106,M107,M108,M109,M110,M111,M112,M113,M114,M115,M116,M117,M118,M119,M120,M121,M122,M123,M124,M125,M126,M127,M128,M129,M130,M131,M132,M133,M134,M135,M136,M137,M138,M139,M140,M141,M142,M143,M144,M145,M146,M147,M148,M149,M150)</f>
-        <v>#NUM!</v>
+        <v>803C00428000806E003B870080AF003D010080CF005080008036008B8C0080B400BD080080FB00D3E90040A500DF9100804D011B9A0080B700E90500806F0145A80080F401106B0080FD0155B80080FA01811D0040D90144850040EE01426F00801700AD91008078008C9000</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
@@ -1092,7 +1092,7 @@
         <v>15</v>
       </c>
       <c r="C14" s="12">
-        <v>277.5</v>
+        <v>253.5</v>
       </c>
       <c r="D14">
         <v>341.5</v>
@@ -1108,9 +1108,9 @@
         <f>IF(B14='Support Data'!$B$4, 'Support Data'!$C$4, 'Support Data'!$C$3)</f>
         <v>80</v>
       </c>
-      <c r="J14" t="e">
+      <c r="J14" t="str">
         <f t="shared" si="1"/>
-        <v>#NUM!</v>
+        <v>FD</v>
       </c>
       <c r="K14" t="str">
         <f t="shared" si="2"/>
@@ -1120,9 +1120,9 @@
         <f t="shared" si="3"/>
         <v>B8</v>
       </c>
-      <c r="M14" t="e">
+      <c r="M14" t="str">
         <f>CONCATENATE(I14,J14,'Support Data'!$C$7,K14,L14,'Support Data'!$C$8)</f>
-        <v>#NUM!</v>
+        <v>80FD0155B800</v>
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
@@ -1133,7 +1133,7 @@
         <v>15</v>
       </c>
       <c r="C15" s="12">
-        <v>263.5</v>
+        <v>250.5</v>
       </c>
       <c r="D15">
         <v>385.5</v>
@@ -1149,9 +1149,9 @@
         <f>IF(B15='Support Data'!$B$4, 'Support Data'!$C$4, 'Support Data'!$C$3)</f>
         <v>80</v>
       </c>
-      <c r="J15" t="e">
+      <c r="J15" t="str">
         <f t="shared" si="1"/>
-        <v>#NUM!</v>
+        <v>FA</v>
       </c>
       <c r="K15" t="str">
         <f t="shared" si="2"/>
@@ -1161,9 +1161,9 @@
         <f t="shared" si="3"/>
         <v>1D</v>
       </c>
-      <c r="M15" t="e">
+      <c r="M15" t="str">
         <f>CONCATENATE(I15,J15,'Support Data'!$C$7,K15,L15,'Support Data'!$C$8)</f>
-        <v>#NUM!</v>
+        <v>80FA01811D00</v>
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
@@ -1357,9 +1357,9 @@
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="e">
+      <c r="A2" t="str">
         <f>'Collected Minutiae'!Q2</f>
-        <v>#NUM!</v>
+        <v>464D5200203230000000008A0000012C019000C500C5010000105B12803C00428000806E003B870080AF003D010080CF005080008036008B8C0080B400BD080080FB00D3E90040A500DF9100804D011B9A0080B700E90500806F0145A80080F401106B0080FD0155B80080FA01811D0040D90144850040EE01426F00801700AD91008078008C90000000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>